<commit_message>
Implement TariffManager class with view, add, delete, and export functions.
</commit_message>
<xml_diff>
--- a/exports/Tariff_Rates_22_06_2025.xlsx
+++ b/exports/Tariff_Rates_22_06_2025.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,63 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Melbourne</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Shanghai</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>40REHC</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Collect</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>14 Days</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
centralise export headers to EXPORT_HEADERS constant.
</commit_message>
<xml_diff>
--- a/exports/Tariff_Rates_22_06_2025.xlsx
+++ b/exports/Tariff_Rates_22_06_2025.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,42 +516,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Taichung</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20GP</t>
+          <t>40GP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>400</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>400</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>120</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>400</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>400</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>400</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -560,63 +560,6 @@
         </is>
       </c>
       <c r="K4" t="inlineStr">
-        <is>
-          <t>14 Days</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Melbourne</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Shanghai</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>40REHC</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Collect</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
         <is>
           <t>14 Days</t>
         </is>

</xml_diff>

<commit_message>
Add import tariff function with validation & update rate prompts to use TariffManager constants.
</commit_message>
<xml_diff>
--- a/exports/Tariff_Rates_22_06_2025.xlsx
+++ b/exports/Tariff_Rates_22_06_2025.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,12 +511,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Melbourne</t>
+          <t>MELBOURNE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Taichung</t>
+          <t>TAICHUNG</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -534,32 +534,267 @@
           <t>400</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>120</v>
+      </c>
+      <c r="G4" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I4" t="n">
+        <v>70</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Collect</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>14 Days</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SYDNEY</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TAICHUNG</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>40GP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>400</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="F5" t="n">
+        <v>120</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20</v>
+      </c>
+      <c r="H5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I5" t="n">
+        <v>70</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Collect</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>14 Days</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BRISBANE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TAICHUNG</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>40GP</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>400</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="F6" t="n">
+        <v>120</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" t="n">
+        <v>30</v>
+      </c>
+      <c r="I6" t="n">
+        <v>70</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Collect</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>14 Days</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TAICHUNG</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>40GP</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>400</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="F7" t="n">
+        <v>120</v>
+      </c>
+      <c r="G7" t="n">
+        <v>20</v>
+      </c>
+      <c r="H7" t="n">
+        <v>30</v>
+      </c>
+      <c r="I7" t="n">
+        <v>70</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Collect</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>14 Days</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MELBOURNE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SHANGHAI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>40GP</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>400</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="F8" t="n">
+        <v>120</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" t="n">
+        <v>30</v>
+      </c>
+      <c r="I8" t="n">
+        <v>70</v>
+      </c>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Collect</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>14 Days</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MELBOURNE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TOKYO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>40GP</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>800</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>120</v>
+      </c>
+      <c r="G9" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" t="n">
+        <v>30</v>
+      </c>
+      <c r="I9" t="n">
+        <v>70</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Collect</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>14 Days</t>
         </is>

</xml_diff>